<commit_message>
Introduced Spring contex for DI.
</commit_message>
<xml_diff>
--- a/src/main/resources/food.xlsx
+++ b/src/main/resources/food.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{F5D2407D-A545-4E20-90B4-1084FD461C88}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="60" windowWidth="11295" windowHeight="5580" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="60" windowWidth="11295" windowHeight="5580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Launch" sheetId="1" r:id="rId1"/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Polish</t>
   </si>
@@ -57,13 +58,28 @@
   </si>
   <si>
     <t>Stinger</t>
+  </si>
+  <si>
+    <t>Cuisines country</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Course</t>
+  </si>
+  <si>
+    <t>Dessert</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Price $</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,15 +96,21 @@
       <charset val="238"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -96,19 +118,64 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -155,7 +222,7 @@
     </a:clrScheme>
     <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -187,9 +254,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -221,6 +306,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Pakiet Office">
@@ -396,58 +499,74 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D1">
+      <c r="D2">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D2">
+      <c r="D3">
         <v>11.25</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="D3">
+      <c r="D4">
         <v>23</v>
       </c>
     </row>
@@ -458,55 +577,63 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B1">
+      <c r="B2">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2">
+      <c r="B3">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>16</v>
       </c>
     </row>

</xml_diff>